<commit_message>
Changes into mutations method
</commit_message>
<xml_diff>
--- a/TransporteSerieNacionalFX/bin/files/Data.xlsx
+++ b/TransporteSerieNacionalFX/bin/files/Data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Infor\GrupoInvestigacion\4to\TransporteSerieNacionalFX\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E860C02D-4218-4397-ACA6-A358E0FA0531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{908165CF-67BF-4669-840E-76A56DDEEA6E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Distancias entre las sedes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,13 +119,13 @@
     <t>Santiago de Cuba</t>
   </si>
   <si>
-    <t>Guántanamo</t>
+    <t>Guantánamo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,19 +498,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369D05D6-3B75-40C9-B009-3921BFCA3FC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -614,7 +613,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -667,7 +666,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -720,7 +719,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -773,7 +772,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -826,7 +825,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -879,7 +878,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -932,7 +931,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -976,7 +975,7 @@
         <v>402</v>
       </c>
       <c r="O9">
-        <v>325</v>
+        <v>400</v>
       </c>
       <c r="P9">
         <v>522</v>
@@ -985,7 +984,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1037,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1143,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1197,7 +1196,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1276,7 +1275,7 @@
         <v>550</v>
       </c>
       <c r="I15">
-        <v>325</v>
+        <v>400</v>
       </c>
       <c r="J15">
         <v>485</v>
@@ -1303,7 +1302,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Added caledarConfiguration class to logic
</commit_message>
<xml_diff>
--- a/TransporteSerieNacionalFX/bin/files/Data.xlsx
+++ b/TransporteSerieNacionalFX/bin/files/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\SNB\TransporteSerieNacionalFX\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFCB758-4823-4CD0-A150-8C6F5C8645CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FCD596-1A84-41A7-9661-4754CFECAE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +511,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,8 +560,17 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -614,7 +623,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -667,7 +676,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -720,7 +729,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -773,7 +782,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -826,7 +835,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -879,7 +888,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -932,7 +941,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -985,7 +994,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1153,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1303,7 +1312,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1419,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="s1EjxOWRyVOLOy6c3eCuaslc5mI7Q1lXsr2AnAfuZdwKZcoUIcndwebHzXMVIV7MrkDrntcp8YBqUX//BpiDSg==" saltValue="RMsDpv/x0LToHezcmZoefg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="3">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el acrónimo de los_x000a_equipo" promptTitle="Acrónimos de los equipos" sqref="B1:Z1" xr:uid="{2BB70D2A-5F1D-46E4-A333-09933192D084}">
+      <formula1>ISTEXT(B1:Z1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el nombre de los equipos" sqref="A2:A26" xr:uid="{E8426092-A3BA-4860-9114-DDE5D0A25DFB}">
+      <formula1>ISTEXT(A2:A26)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir la distancia entre las sedes de los equipos" sqref="B2:Z26" xr:uid="{EFCFD96C-4502-4865-9FF4-BC5C1FE6F3CD}">
+      <formula1>ISNUMBER(B2:Z26)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed several calendar methods
</commit_message>
<xml_diff>
--- a/TransporteSerieNacionalFX/bin/files/Data.xlsx
+++ b/TransporteSerieNacionalFX/bin/files/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\SNB\TransporteSerieNacionalFX\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FCD596-1A84-41A7-9661-4754CFECAE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DC1318-D589-49F4-9157-2C0760CEAA20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +511,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,17 +560,8 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -623,7 +614,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -676,7 +667,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -729,7 +720,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -782,7 +773,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -835,7 +826,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -888,7 +879,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -941,7 +932,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -994,7 +985,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1047,7 +1038,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1100,7 +1091,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1153,7 +1144,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1206,7 +1197,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1259,7 +1250,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1312,7 +1303,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1420,15 +1411,15 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el acrónimo de los_x000a_equipo" promptTitle="Acrónimos de los equipos" sqref="B1:Z1" xr:uid="{2BB70D2A-5F1D-46E4-A333-09933192D084}">
-      <formula1>ISTEXT(B1:Z1)</formula1>
-    </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el nombre de los equipos" sqref="A2:A26" xr:uid="{E8426092-A3BA-4860-9114-DDE5D0A25DFB}">
       <formula1>ISTEXT(A2:A26)</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir la distancia entre las sedes de los equipos" sqref="B2:Z26" xr:uid="{EFCFD96C-4502-4865-9FF4-BC5C1FE6F3CD}">
       <formula1>ISNUMBER(B2:Z26)</formula1>
     </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el acrónimo de los_x000a_equipo" promptTitle="Acrónimos de los equipos" sqref="B1:Q1" xr:uid="{2BB70D2A-5F1D-46E4-A333-09933192D084}">
+      <formula1>ISTEXT(B1:Q1)</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>